<commit_message>
Updated EntityModifierBenchmark to make use of SpriteBatch(SpriteGroup).
</commit_message>
<xml_diff>
--- a/doc/spritebatch_benchmark.xlsx
+++ b/doc/spritebatch_benchmark.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr showPivotChartFilter="1" defaultThemeVersion="124226"/>
+  <workbookPr hidePivotFieldList="1" showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="27315" windowHeight="13095"/>
   </bookViews>
@@ -16,11 +16,12 @@
   <pivotCaches>
     <pivotCache cacheId="12" r:id="rId5"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Nexus One</t>
   </si>
@@ -95,6 +96,24 @@
   </si>
   <si>
     <t xml:space="preserve">Sprites (Shared VertexBuffer) </t>
+  </si>
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>SpriteBenchmark</t>
+  </si>
+  <si>
+    <t>EntityModifierBenchmark</t>
+  </si>
+  <si>
+    <t>LG Optimus 3D</t>
+  </si>
+  <si>
+    <t>2.2.2</t>
+  </si>
+  <si>
+    <t>LG Optimus 3D (2.2.2)</t>
   </si>
 </sst>
 </file>
@@ -332,7 +351,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="244">
+  <dxfs count="90">
     <dxf>
       <fill>
         <patternFill>
@@ -856,11 +875,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor auto="1"/>
@@ -943,6 +957,11 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor auto="1"/>
@@ -1025,31 +1044,21 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment textRotation="66" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
+      <font>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -1100,1425 +1109,10 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment textRotation="45" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment textRotation="66" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment textRotation="67" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment textRotation="67" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment textRotation="67" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment textRotation="67" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment textRotation="67" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment textRotation="67" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment textRotation="67" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment textRotation="67" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment textRotation="67" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment textRotation="67" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -2825,25 +1419,75 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Benchmark!$H$3:$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LG Optimus 3D (2.2.2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Benchmark!$B$5:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Sprites </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprites (Shared VertexBuffer) </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SpriteBatch </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Benchmark!$H$5:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>36.159999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="99939456"/>
-        <c:axId val="100057472"/>
+        <c:axId val="51709440"/>
+        <c:axId val="51710976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99939456"/>
+        <c:axId val="51709440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100057472"/>
+        <c:crossAx val="51710976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100057472"/>
+        <c:axId val="51710976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2851,7 +1495,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99939456"/>
+        <c:crossAx val="51709440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2869,7 +1513,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2880,13 +1524,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>314326</xdr:colOff>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
+      <xdr:colOff>1255058</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
@@ -2911,41 +1555,49 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Nicolas Gramlich" refreshedDate="40708.877357291669" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="5">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Nicolas Gramlich" refreshedDate="40709.559959953702" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="12">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:E6" sheet="Data"/>
+    <worksheetSource ref="A1:F13" sheet="Data"/>
   </cacheSource>
-  <cacheFields count="5">
+  <cacheFields count="6">
     <cacheField name="Model" numFmtId="0">
-      <sharedItems count="5">
+      <sharedItems count="6">
         <s v="Nexus One"/>
         <s v="HTC Tattoo"/>
         <s v="Xperia Play"/>
         <s v="Samsung Galaxy Tab 10.1"/>
+        <s v="LG Optimus 3D"/>
         <s v="Motorola Xoom"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Android Version" numFmtId="49">
       <sharedItems/>
     </cacheField>
+    <cacheField name="Benchmark" numFmtId="49">
+      <sharedItems count="2">
+        <s v="SpriteBenchmark"/>
+        <s v="EntityModifierBenchmark"/>
+      </sharedItems>
+    </cacheField>
     <cacheField name="Sprites" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.49" maxValue="29.85"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.66" maxValue="36.159999999999997"/>
     </cacheField>
     <cacheField name="Sprites (Shared VertexBuffer)" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.95" maxValue="36.5"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.87" maxValue="46.2"/>
     </cacheField>
     <cacheField name="SpriteBatch" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="7.54" maxValue="59.24"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.69" maxValue="59.24"/>
     </cacheField>
   </cacheFields>
 </pivotCacheDefinition>
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="5">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="12">
   <r>
     <x v="0"/>
     <s v="2.3.4"/>
+    <x v="0"/>
     <n v="19.98"/>
     <n v="23.8"/>
     <n v="45.1"/>
@@ -2953,6 +1605,7 @@
   <r>
     <x v="1"/>
     <s v="1.6"/>
+    <x v="0"/>
     <n v="3.49"/>
     <n v="3.95"/>
     <n v="7.54"/>
@@ -2960,6 +1613,7 @@
   <r>
     <x v="2"/>
     <s v="2.3.2"/>
+    <x v="0"/>
     <n v="23.4"/>
     <n v="26.14"/>
     <n v="59.24"/>
@@ -2967,35 +1621,100 @@
   <r>
     <x v="3"/>
     <s v="3.1"/>
+    <x v="0"/>
     <n v="29.85"/>
     <n v="36.5"/>
     <n v="56.5"/>
   </r>
   <r>
     <x v="4"/>
+    <s v="2.2.2"/>
+    <x v="0"/>
+    <n v="36.159999999999997"/>
+    <n v="46.2"/>
+    <n v="58.01"/>
+  </r>
+  <r>
+    <x v="5"/>
     <s v="3.0.1"/>
+    <x v="0"/>
     <n v="29.84"/>
     <n v="36.14"/>
     <n v="47.64"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2.3.4"/>
+    <x v="1"/>
+    <n v="14.15"/>
+    <n v="15.54"/>
+    <n v="32.01"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="1.6"/>
+    <x v="1"/>
+    <n v="2.66"/>
+    <n v="2.87"/>
+    <n v="2.69"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2.3.2"/>
+    <x v="1"/>
+    <n v="17.27"/>
+    <n v="18.75"/>
+    <n v="40.46"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="3.1"/>
+    <x v="1"/>
+    <n v="22.92"/>
+    <n v="22.77"/>
+    <n v="29.41"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="3.0.1"/>
+    <x v="1"/>
+    <n v="22.9"/>
+    <n v="22.52"/>
+    <n v="29.49"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="2.2.2"/>
+    <x v="1"/>
+    <n v="19.440000000000001"/>
+    <n v="22.46"/>
+    <n v="41.67"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption=" " updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="  " colHeaderCaption="     ">
-  <location ref="B3:G7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption=" " updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="  " colHeaderCaption="     ">
+  <location ref="B3:H7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="6">
     <pivotField axis="axisCol" showAll="0">
-      <items count="6">
+      <items count="7">
         <item n="HTC Tattoo (1.6)" sd="0" x="1"/>
         <item n="Nexus One (2.3.4)" sd="0" x="0"/>
         <item n="Xperia Play (2.3.2)" sd="0" x="2"/>
-        <item n="Motorola Xoom (3.0.1)" sd="0" x="4"/>
+        <item n="Motorola Xoom (3.0.1)" sd="0" x="5"/>
         <item n="Samsung Galaxy Tab 10.1 (3.1)" sd="0" x="3"/>
+        <item n="LG Optimus 3D (2.2.2)" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="0"/>
+        <item h="1" x="1"/>
+      </items>
+    </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -3017,7 +1736,7 @@
   <colFields count="1">
     <field x="0"/>
   </colFields>
-  <colItems count="5">
+  <colItems count="6">
     <i>
       <x/>
     </i>
@@ -3033,47 +1752,53 @@
     <i>
       <x v="4"/>
     </i>
+    <i>
+      <x v="5"/>
+    </i>
   </colItems>
+  <pageFields count="1">
+    <pageField fld="2" hier="-1"/>
+  </pageFields>
   <dataFields count="3">
-    <dataField name="Sprites " fld="2" baseField="0" baseItem="0"/>
-    <dataField name="Sprites (Shared VertexBuffer) " fld="3" baseField="0" baseItem="0"/>
-    <dataField name="SpriteBatch " fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sprites " fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Sprites (Shared VertexBuffer) " fld="4" baseField="0" baseItem="0"/>
+    <dataField name="SpriteBatch " fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="10">
-    <format dxfId="243">
+    <format dxfId="89">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="242">
+    <format dxfId="88">
       <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="241">
+    <format dxfId="87">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="98">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="94">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="83">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="90">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -3084,14 +1809,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="81">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="60">
+    <format dxfId="80">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="20">
+  <chartFormats count="21">
     <chartFormat chart="2" format="4" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -3283,6 +2008,18 @@
           </reference>
           <reference field="0" count="1" selected="0">
             <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
           </reference>
         </references>
       </pivotArea>
@@ -3577,19 +2314,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:G19"/>
+  <dimension ref="B1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" customWidth="1"/>
-    <col min="4" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="8" width="6.140625" customWidth="1"/>
     <col min="9" max="9" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.28515625" customWidth="1"/>
     <col min="11" max="11" width="27.7109375" customWidth="1"/>
@@ -3600,7 +2335,15 @@
     <col min="16" max="16" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1">
+    <row r="1" spans="2:8">
+      <c r="B1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="15.75" thickBot="1">
       <c r="B3" s="4"/>
       <c r="C3" s="3" t="s">
         <v>22</v>
@@ -3609,8 +2352,9 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="2:7" ht="136.5" thickBot="1">
+    <row r="4" spans="2:8" ht="136.5" thickBot="1">
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
@@ -3626,11 +2370,14 @@
       <c r="F4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="H4" s="10" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:8">
       <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
@@ -3646,11 +2393,14 @@
       <c r="F5" s="12">
         <v>29.84</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <v>29.85</v>
       </c>
+      <c r="H5" s="13">
+        <v>36.159999999999997</v>
+      </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:8">
       <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
@@ -3666,11 +2416,14 @@
       <c r="F6" s="15">
         <v>36.14</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="15">
         <v>36.5</v>
       </c>
+      <c r="H6" s="16">
+        <v>46.2</v>
+      </c>
     </row>
-    <row r="7" spans="2:7" ht="15.75" thickBot="1">
+    <row r="7" spans="2:8" ht="15.75" thickBot="1">
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
@@ -3686,12 +2439,15 @@
       <c r="F7" s="18">
         <v>47.64</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="18">
         <v>56.5</v>
       </c>
+      <c r="H7" s="19">
+        <v>58.01</v>
+      </c>
     </row>
-    <row r="10" spans="2:7" ht="15.75" thickBot="1"/>
-    <row r="14" spans="2:7" ht="15.75" thickBot="1"/>
+    <row r="10" spans="2:8" ht="15.75" thickBot="1"/>
+    <row r="14" spans="2:8" ht="15.75" thickBot="1"/>
     <row r="19" ht="15.75" thickBot="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3701,20 +2457,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3722,98 +2479,256 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
         <v>19.98</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>23.8</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>45.1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
         <v>3.49</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3.95</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>7.54</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
         <v>23.4</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>26.14</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>59.24</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
         <v>29.85</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>36.5</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>56.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>36.159999999999997</v>
+      </c>
+      <c r="E6">
+        <v>46.2</v>
+      </c>
+      <c r="F6">
+        <v>58.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6">
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7">
         <v>29.84</v>
       </c>
-      <c r="D6">
+      <c r="E7">
         <v>36.14</v>
       </c>
-      <c r="E6">
+      <c r="F7">
         <v>47.64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>14.15</v>
+      </c>
+      <c r="E8">
+        <v>15.54</v>
+      </c>
+      <c r="F8">
+        <v>32.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>2.66</v>
+      </c>
+      <c r="E9">
+        <v>2.87</v>
+      </c>
+      <c r="F9">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10">
+        <v>17.27</v>
+      </c>
+      <c r="E10">
+        <v>18.75</v>
+      </c>
+      <c r="F10">
+        <v>40.46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>22.92</v>
+      </c>
+      <c r="E11">
+        <v>22.77</v>
+      </c>
+      <c r="F11">
+        <v>29.41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>22.9</v>
+      </c>
+      <c r="E12">
+        <v>22.52</v>
+      </c>
+      <c r="F12">
+        <v>29.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>19.440000000000001</v>
+      </c>
+      <c r="E13">
+        <v>22.46</v>
+      </c>
+      <c r="F13">
+        <v>41.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>